<commit_message>
update benchmark excel with cost graphs
</commit_message>
<xml_diff>
--- a/results/aws-postgres-benchmark.xlsx
+++ b/results/aws-postgres-benchmark.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aviitala/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aviitala/dev-personal/aws-aurora-vs-rds-performance-benchmark/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E486124E-C344-A046-A10C-A12210AD2150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA00AD2-496F-0D4F-B669-1C929B3CC81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="26800" xr2:uid="{3B69575C-2310-7346-8623-959C48E2B592}"/>
+    <workbookView xWindow="28260" yWindow="500" windowWidth="40540" windowHeight="26800" activeTab="1" xr2:uid="{3B69575C-2310-7346-8623-959C48E2B592}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Performance" sheetId="1" r:id="rId1"/>
+    <sheet name="Costs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>Iteration</t>
   </si>
@@ -80,11 +84,49 @@
     <t>Iteration 4
 (no RDS bursting)</t>
   </si>
+  <si>
+    <t>DB Size</t>
+  </si>
+  <si>
+    <t>I/O per second (IOPS)</t>
+  </si>
+  <si>
+    <t>RDS</t>
+  </si>
+  <si>
+    <t>Aurora Standard</t>
+  </si>
+  <si>
+    <t>Aurora I/O-optimized</t>
+  </si>
+  <si>
+    <t>Baseline cost per month</t>
+  </si>
+  <si>
+    <t>EC2</t>
+  </si>
+  <si>
+    <t>Storage per GB</t>
+  </si>
+  <si>
+    <t>Per IO</t>
+  </si>
+  <si>
+    <t>Per IOPS, per month</t>
+  </si>
+  <si>
+    <t>Aurora I/O optimized</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00000000000_);_([$$-409]* \(#,##0.00000000000\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -187,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -205,6 +247,12 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,9 +261,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF5CCF"/>
+      <color rgb="FF0CCFE7"/>
+      <color rgb="FFFF7E00"/>
+      <color rgb="FFFF00C6"/>
       <color rgb="FF3A3A3A"/>
-      <color rgb="FFFF7E00"/>
-      <color rgb="FF0CCFE7"/>
     </mruColors>
   </colors>
   <extLst>
@@ -304,7 +354,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>Performance!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -380,7 +430,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$E$3</c:f>
+              <c:f>Performance!$B$3:$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -404,7 +454,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$E$4</c:f>
+              <c:f>Performance!$B$4:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -434,7 +484,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>Performance!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -510,7 +560,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$E$3</c:f>
+              <c:f>Performance!$B$3:$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -534,7 +584,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$E$5</c:f>
+              <c:f>Performance!$B$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -888,7 +938,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
+              <c:f>Performance!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -964,7 +1014,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$E$3</c:f>
+              <c:f>Performance!$B$3:$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -988,7 +1038,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$E$9</c:f>
+              <c:f>Performance!$B$9:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1018,7 +1068,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$10</c:f>
+              <c:f>Performance!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1094,7 +1144,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$E$3</c:f>
+              <c:f>Performance!$B$3:$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1118,7 +1168,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$E$10</c:f>
+              <c:f>Performance!$B$10:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1472,7 +1522,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$14</c:f>
+              <c:f>Performance!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1548,7 +1598,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$E$3</c:f>
+              <c:f>Performance!$B$3:$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1572,7 +1622,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$E$14</c:f>
+              <c:f>Performance!$B$14:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1602,7 +1652,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
+              <c:f>Performance!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1678,7 +1728,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$E$3</c:f>
+              <c:f>Performance!$B$3:$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1702,7 +1752,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$E$15</c:f>
+              <c:f>Performance!$B$15:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1972,6 +2022,2023 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" i="0" baseline="0"/>
+              <a:t>Total cost for 100 GB database</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1050" i="0" baseline="0"/>
+              <a:t>USD per year, on-demand, 1x </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>r6g.large</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1050" i="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1142553290532561"/>
+          <c:y val="0.19789689931364191"/>
+          <c:w val="0.67541286293294966"/>
+          <c:h val="0.62669525790710312"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Costs!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0CCFE7"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Costs!$A$8:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Costs!$B$8:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2530.8000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2530.8000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2530.8000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2530.8000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2530.8000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2530.8000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2530.8000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7C6A-FC4B-BF56-624F790EA3E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Costs!$C$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aurora Standard</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF5CCF"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Costs!$A$8:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Costs!$C$8:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2832.81792</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3172.7760000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3519.6720000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3866.5680000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4213.4639999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4560.3599999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4907.2559999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7C6A-FC4B-BF56-624F790EA3E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Costs!$D$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aurora I/O-optimized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF7E00"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Costs!$A$8:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Costs!$D$8:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3862.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3862.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3862.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3862.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3862.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3862.92</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3862.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7C6A-FC4B-BF56-624F790EA3E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="680127728"/>
+        <c:axId val="680130256"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="680127728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Constant</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> IOPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.38162640384237684"/>
+              <c:y val="0.91341851944432872"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="680130256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="680130256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="680127728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82055288369566048"/>
+          <c:y val="0.29275526713969113"/>
+          <c:w val="0.16237016929006323"/>
+          <c:h val="0.42737850827015872"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="3A3A3A"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" i="0" baseline="0"/>
+              <a:t>Total cost for 300 GB database</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1050" i="0" baseline="0"/>
+              <a:t>USD per year, on-demand, 1x r6g.large</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1050" i="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1142553290532561"/>
+          <c:y val="0.19789689931364191"/>
+          <c:w val="0.67541286293294966"/>
+          <c:h val="0.62669525790710312"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Costs!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0CCFE7"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Costs!$A$20:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Costs!$B$20:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2862</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2862</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2862</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2862</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2862</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2862</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2862</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2862</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2862</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2862</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6F24-944E-AFC7-82D6A8D0BD27}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Costs!$C$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aurora Standard</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF5CCF"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Costs!$A$20:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Costs!$C$20:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3096.8179200000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3783.6720000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4477.4639999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5171.2559999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5865.0480000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6558.8399999999992</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7252.6319999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7946.424</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8640.2160000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9334.0080000000016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6F24-944E-AFC7-82D6A8D0BD27}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Costs!$D$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aurora I/O-optimized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF7E00"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Costs!$A$20:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Costs!$D$20:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4458.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4458.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4458.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4458.12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4458.12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4458.12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4458.12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4458.12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4458.12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4458.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6F24-944E-AFC7-82D6A8D0BD27}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="680127728"/>
+        <c:axId val="680130256"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="680127728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Constant</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> IOPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.38162640384237684"/>
+              <c:y val="0.91341851944432872"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="680130256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="680130256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="680127728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2000"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82055288369566048"/>
+          <c:y val="0.29275526713969113"/>
+          <c:w val="0.16237016929006323"/>
+          <c:h val="0.42737850827015872"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="3A3A3A"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" i="0" baseline="0"/>
+              <a:t>Total cost for 1000 GB database</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1050" i="0" baseline="0"/>
+              <a:t>USD per year, on-demand, </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>1x r6g.large</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1142553290532561"/>
+          <c:y val="0.19789689931364191"/>
+          <c:w val="0.67541286293294966"/>
+          <c:h val="0.62669525790710312"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Costs!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0CCFE7"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Costs!$A$35:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Costs!$B$35:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4021.2000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4021.2000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4021.2000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4021.2000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4021.2000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4021.2000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4021.2000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FB81-C943-8E2C-5D8AA814267D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Costs!$C$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aurora Standard</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF5CCF"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Costs!$A$35:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Costs!$C$35:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4020.8179200000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7482.8399999999992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10951.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14420.76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17889.72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21358.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24827.640000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FB81-C943-8E2C-5D8AA814267D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Costs!$D$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aurora I/O-optimized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF7E00"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Costs!$A$35:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Costs!$D$35:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6541.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6541.32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6541.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6541.32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6541.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6541.32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6541.32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FB81-C943-8E2C-5D8AA814267D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="680127728"/>
+        <c:axId val="680130256"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="680127728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Constant</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> IOPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.38162640384237684"/>
+              <c:y val="0.91341851944432872"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="680130256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="680130256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="680127728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82055288369566048"/>
+          <c:y val="0.29275526713969113"/>
+          <c:w val="0.16237016929006323"/>
+          <c:h val="0.42737850827015872"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="3A3A3A"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2092,6 +4159,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3248,6 +5435,1554 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3606,15 +7341,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>459447</xdr:colOff>
+      <xdr:colOff>450376</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>50249</xdr:rowOff>
+      <xdr:rowOff>41178</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1286761</xdr:colOff>
+      <xdr:colOff>1274796</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>79277</xdr:rowOff>
+      <xdr:rowOff>68610</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3718,6 +7453,237 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>623930</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>53553</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>286593</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>189623</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{896E4BFC-9CBE-9B40-B0C4-8BFE091472D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>612048</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>191266</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>274711</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>120770</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8452ED7-10D1-5C42-B73A-F04738779BF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>650301</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>7651</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>312964</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>159022</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5281F78-92FD-0E44-BB45-9515A1199EA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>RDS</v>
+          </cell>
+          <cell r="C2" t="str">
+            <v>Aurora Standard</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>Aurora I/O-optimized</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>1</v>
+          </cell>
+          <cell r="B3">
+            <v>210.9</v>
+          </cell>
+          <cell r="C3">
+            <v>236.06816000000001</v>
+          </cell>
+          <cell r="D3">
+            <v>321.91000000000003</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>25</v>
+          </cell>
+          <cell r="B4">
+            <v>210.9</v>
+          </cell>
+          <cell r="C4">
+            <v>249.94400000000002</v>
+          </cell>
+          <cell r="D4">
+            <v>321.91000000000003</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>50</v>
+          </cell>
+          <cell r="B5">
+            <v>210.9</v>
+          </cell>
+          <cell r="C5">
+            <v>264.39800000000002</v>
+          </cell>
+          <cell r="D5">
+            <v>321.91000000000003</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>100</v>
+          </cell>
+          <cell r="B6">
+            <v>210.9</v>
+          </cell>
+          <cell r="C6">
+            <v>293.30600000000004</v>
+          </cell>
+          <cell r="D6">
+            <v>321.91000000000003</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>250</v>
+          </cell>
+          <cell r="B7">
+            <v>210.9</v>
+          </cell>
+          <cell r="C7">
+            <v>380.03</v>
+          </cell>
+          <cell r="D7">
+            <v>321.91000000000003</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>300</v>
+          </cell>
+          <cell r="B8">
+            <v>210.9</v>
+          </cell>
+          <cell r="C8">
+            <v>408.93799999999999</v>
+          </cell>
+          <cell r="D8">
+            <v>321.91000000000003</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4019,9 +7985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51763E1-694A-DE44-BFAB-A7E90165BDCB}">
   <dimension ref="A2:E15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4220,4 +8184,602 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A699B5F9-1686-614D-AD85-4C7B4C7D864E}">
+  <dimension ref="A1:E44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="14">
+        <v>197.1</v>
+      </c>
+      <c r="C2" s="15">
+        <f>13.8/100</f>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D2" s="15">
+        <v>0</v>
+      </c>
+      <c r="E2" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="14">
+        <v>224.49</v>
+      </c>
+      <c r="C3" s="15">
+        <f>11/100</f>
+        <v>0.11</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2.2000000000000001E-7</v>
+      </c>
+      <c r="E3" s="14">
+        <f>D3*60*60*730</f>
+        <v>0.57816000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="14">
+        <v>297.11</v>
+      </c>
+      <c r="C4" s="15">
+        <f>24.8/100</f>
+        <v>0.248</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="16">
+        <f>(B$2+$C$2*$B$6)*12</f>
+        <v>2530.8000000000002</v>
+      </c>
+      <c r="C8" s="16">
+        <f>($B$3+$C$3*$B$6+A8*$E$3)*12</f>
+        <v>2832.81792</v>
+      </c>
+      <c r="D8" s="16">
+        <f>($B$4+$C$4*$B$6+A8*$E$4)*12</f>
+        <v>3862.92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9" s="16">
+        <f t="shared" ref="B9:B14" si="0">(B$2+$C$2*$B$6)*12</f>
+        <v>2530.8000000000002</v>
+      </c>
+      <c r="C9" s="16">
+        <f t="shared" ref="C9:C14" si="1">($B$3+$C$3*$B$6+A9*$E$3)*12</f>
+        <v>3172.7760000000003</v>
+      </c>
+      <c r="D9" s="16">
+        <f t="shared" ref="D9:D14" si="2">($B$4+$C$4*$B$6+A9*$E$4)*12</f>
+        <v>3862.92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="B10" s="16">
+        <f t="shared" si="0"/>
+        <v>2530.8000000000002</v>
+      </c>
+      <c r="C10" s="16">
+        <f t="shared" si="1"/>
+        <v>3519.6720000000005</v>
+      </c>
+      <c r="D10" s="16">
+        <f t="shared" si="2"/>
+        <v>3862.92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>150</v>
+      </c>
+      <c r="B11" s="16">
+        <f t="shared" si="0"/>
+        <v>2530.8000000000002</v>
+      </c>
+      <c r="C11" s="16">
+        <f t="shared" si="1"/>
+        <v>3866.5680000000002</v>
+      </c>
+      <c r="D11" s="16">
+        <f t="shared" si="2"/>
+        <v>3862.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>200</v>
+      </c>
+      <c r="B12" s="16">
+        <f t="shared" si="0"/>
+        <v>2530.8000000000002</v>
+      </c>
+      <c r="C12" s="16">
+        <f t="shared" si="1"/>
+        <v>4213.4639999999999</v>
+      </c>
+      <c r="D12" s="16">
+        <f t="shared" si="2"/>
+        <v>3862.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>250</v>
+      </c>
+      <c r="B13" s="16">
+        <f t="shared" si="0"/>
+        <v>2530.8000000000002</v>
+      </c>
+      <c r="C13" s="16">
+        <f t="shared" si="1"/>
+        <v>4560.3599999999997</v>
+      </c>
+      <c r="D13" s="16">
+        <f t="shared" si="2"/>
+        <v>3862.92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>300</v>
+      </c>
+      <c r="B14" s="16">
+        <f t="shared" si="0"/>
+        <v>2530.8000000000002</v>
+      </c>
+      <c r="C14" s="16">
+        <f t="shared" si="1"/>
+        <v>4907.2559999999994</v>
+      </c>
+      <c r="D14" s="16">
+        <f t="shared" si="2"/>
+        <v>3862.92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="16">
+        <f>(B$2+$C$2*$B$18)*12</f>
+        <v>2862</v>
+      </c>
+      <c r="C20" s="16">
+        <f>($B$3+$C$3*$B$18+A20*$E$3)*12</f>
+        <v>3096.8179200000004</v>
+      </c>
+      <c r="D20" s="16">
+        <f>($B$4+$C$4*$B$18+A20*$E$4)*12</f>
+        <v>4458.12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>100</v>
+      </c>
+      <c r="B21" s="16">
+        <f t="shared" ref="B21:B29" si="3">(B$2+$C$2*$B$18)*12</f>
+        <v>2862</v>
+      </c>
+      <c r="C21" s="16">
+        <f t="shared" ref="C21:C29" si="4">($B$3+$C$3*$B$18+A21*$E$3)*12</f>
+        <v>3783.6720000000005</v>
+      </c>
+      <c r="D21" s="16">
+        <f t="shared" ref="D21:D29" si="5">($B$4+$C$4*$B$18+A21*$E$4)*12</f>
+        <v>4458.12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>200</v>
+      </c>
+      <c r="B22" s="16">
+        <f t="shared" si="3"/>
+        <v>2862</v>
+      </c>
+      <c r="C22" s="16">
+        <f t="shared" si="4"/>
+        <v>4477.4639999999999</v>
+      </c>
+      <c r="D22" s="16">
+        <f t="shared" si="5"/>
+        <v>4458.12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>300</v>
+      </c>
+      <c r="B23" s="16">
+        <f t="shared" si="3"/>
+        <v>2862</v>
+      </c>
+      <c r="C23" s="16">
+        <f t="shared" si="4"/>
+        <v>5171.2559999999994</v>
+      </c>
+      <c r="D23" s="16">
+        <f t="shared" si="5"/>
+        <v>4458.12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>400</v>
+      </c>
+      <c r="B24" s="16">
+        <f t="shared" si="3"/>
+        <v>2862</v>
+      </c>
+      <c r="C24" s="16">
+        <f t="shared" si="4"/>
+        <v>5865.0480000000007</v>
+      </c>
+      <c r="D24" s="16">
+        <f t="shared" si="5"/>
+        <v>4458.12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>500</v>
+      </c>
+      <c r="B25" s="16">
+        <f t="shared" si="3"/>
+        <v>2862</v>
+      </c>
+      <c r="C25" s="16">
+        <f t="shared" si="4"/>
+        <v>6558.8399999999992</v>
+      </c>
+      <c r="D25" s="16">
+        <f t="shared" si="5"/>
+        <v>4458.12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>600</v>
+      </c>
+      <c r="B26" s="16">
+        <f t="shared" si="3"/>
+        <v>2862</v>
+      </c>
+      <c r="C26" s="16">
+        <f t="shared" si="4"/>
+        <v>7252.6319999999996</v>
+      </c>
+      <c r="D26" s="16">
+        <f t="shared" si="5"/>
+        <v>4458.12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>700</v>
+      </c>
+      <c r="B27" s="16">
+        <f t="shared" si="3"/>
+        <v>2862</v>
+      </c>
+      <c r="C27" s="16">
+        <f t="shared" si="4"/>
+        <v>7946.424</v>
+      </c>
+      <c r="D27" s="16">
+        <f t="shared" si="5"/>
+        <v>4458.12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>800</v>
+      </c>
+      <c r="B28" s="16">
+        <f t="shared" si="3"/>
+        <v>2862</v>
+      </c>
+      <c r="C28" s="16">
+        <f t="shared" si="4"/>
+        <v>8640.2160000000003</v>
+      </c>
+      <c r="D28" s="16">
+        <f t="shared" si="5"/>
+        <v>4458.12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>900</v>
+      </c>
+      <c r="B29" s="16">
+        <f t="shared" si="3"/>
+        <v>2862</v>
+      </c>
+      <c r="C29" s="16">
+        <f t="shared" si="4"/>
+        <v>9334.0080000000016</v>
+      </c>
+      <c r="D29" s="16">
+        <f t="shared" si="5"/>
+        <v>4458.12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" s="16">
+        <f>(B$2+$C$2*$B$33)*12</f>
+        <v>4021.2000000000003</v>
+      </c>
+      <c r="C35" s="16">
+        <f>($B$3+$C$3*$B$33+A35*$E$3)*12</f>
+        <v>4020.8179200000004</v>
+      </c>
+      <c r="D35" s="16">
+        <f>($B$4+$C$4*$B$33+A35*$E$4)*12</f>
+        <v>6541.32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>500</v>
+      </c>
+      <c r="B36" s="16">
+        <f t="shared" ref="B36:B44" si="6">(B$2+$C$2*$B$33)*12</f>
+        <v>4021.2000000000003</v>
+      </c>
+      <c r="C36" s="16">
+        <f t="shared" ref="C36:C44" si="7">($B$3+$C$3*$B$33+A36*$E$3)*12</f>
+        <v>7482.8399999999992</v>
+      </c>
+      <c r="D36" s="16">
+        <f t="shared" ref="D36:D44" si="8">($B$4+$C$4*$B$33+A36*$E$4)*12</f>
+        <v>6541.32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1000</v>
+      </c>
+      <c r="B37" s="16">
+        <f t="shared" si="6"/>
+        <v>4021.2000000000003</v>
+      </c>
+      <c r="C37" s="16">
+        <f t="shared" si="7"/>
+        <v>10951.8</v>
+      </c>
+      <c r="D37" s="16">
+        <f t="shared" si="8"/>
+        <v>6541.32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1500</v>
+      </c>
+      <c r="B38" s="16">
+        <f t="shared" si="6"/>
+        <v>4021.2000000000003</v>
+      </c>
+      <c r="C38" s="16">
+        <f t="shared" si="7"/>
+        <v>14420.76</v>
+      </c>
+      <c r="D38" s="16">
+        <f t="shared" si="8"/>
+        <v>6541.32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2000</v>
+      </c>
+      <c r="B39" s="16">
+        <f t="shared" si="6"/>
+        <v>4021.2000000000003</v>
+      </c>
+      <c r="C39" s="16">
+        <f t="shared" si="7"/>
+        <v>17889.72</v>
+      </c>
+      <c r="D39" s="16">
+        <f t="shared" si="8"/>
+        <v>6541.32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2500</v>
+      </c>
+      <c r="B40" s="16">
+        <f t="shared" si="6"/>
+        <v>4021.2000000000003</v>
+      </c>
+      <c r="C40" s="16">
+        <f t="shared" si="7"/>
+        <v>21358.68</v>
+      </c>
+      <c r="D40" s="16">
+        <f t="shared" si="8"/>
+        <v>6541.32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3000</v>
+      </c>
+      <c r="B41" s="16">
+        <f t="shared" si="6"/>
+        <v>4021.2000000000003</v>
+      </c>
+      <c r="C41" s="16">
+        <f t="shared" si="7"/>
+        <v>24827.640000000003</v>
+      </c>
+      <c r="D41" s="16">
+        <f t="shared" si="8"/>
+        <v>6541.32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>